<commit_message>
google ads and google analytics basic functionality built
loop for customer ids / view ids
both need testing, error handling, additional functionality
</commit_message>
<xml_diff>
--- a/Google Analytics/google_analytics_conf_1.xlsx
+++ b/Google Analytics/google_analytics_conf_1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBE07888-5AC0-4DDD-997C-521CE8D5E14E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4454AA-59F1-4D81-9BF2-0C361F4B261C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,6 @@
     <sheet name="parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -522,7 +521,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:G10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +553,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>